<commit_message>
add get status rotation
</commit_message>
<xml_diff>
--- a/Universal_Driver_soft/UD_v3.1_stepEnc/Map Registers UD3.2 step.xlsx
+++ b/Universal_Driver_soft/UD_v3.1_stepEnc/Map Registers UD3.2 step.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B502B865-AEE6-42D4-B77E-708E06F6DAFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351E33CF-A316-4E7F-AC95-05FC3353F58A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>Десятичная</t>
   </si>
@@ -386,15 +386,6 @@
     <t>C7A0D70N0x</t>
   </si>
   <si>
-    <t xml:space="preserve">C1A0D1N0x
-C1 - комманда
-A0 -
-D1 - 1 старт стартует и крутится до значения указанного в Target или бесконечно
- 0 - принудительный стоп из любого режима
-2- экстренный стоп
-N1 - </t>
-  </si>
-  <si>
     <t>C4A0D1000N0x</t>
   </si>
   <si>
@@ -414,10 +405,6 @@
     <t xml:space="preserve">Новые функции </t>
   </si>
   <si>
-    <t>25.05.2024
-Добавлен экстренный стоп(без торможения)</t>
-  </si>
-  <si>
     <t>Добавлен параметр начальной скорости. С этой скорости начинается разгон</t>
   </si>
   <si>
@@ -450,6 +437,27 @@
 D1 - бесконечн
 D2 - Количество шагов по счетчику
 D3 - Количество шагов по энкодеру</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1A0D1N0x
+C1 - комманда
+A0 -  0 записать 1 прочитать
+D1 - 1 старт стартует и крутится до значения указанного в Target или бесконечно
+ 0 - принудительный стоп из любого режима
+2- экстренный стоп
+N1 - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.05.2024
+Добавлен экстренный стоп(без торможения)
+</t>
+  </si>
+  <si>
+    <t>Возврощаемое значение при A1
+MOTION = 0
+STOPPED = 1
+ACCEL = 2
+BRAKING = 3</t>
   </si>
 </sst>
 </file>
@@ -956,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1011,10 +1019,10 @@
         <v>71</v>
       </c>
       <c r="H3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="189.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1032,12 +1040,14 @@
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" s="6"/>
+        <v>85</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>87</v>
+      </c>
       <c r="H4" s="6"/>
       <c r="I4" s="11" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="156" customHeight="1" x14ac:dyDescent="0.3">
@@ -1078,14 +1088,14 @@
         <v>40</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="129" customHeight="1" x14ac:dyDescent="0.3">
@@ -1109,7 +1119,7 @@
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="229.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1150,7 +1160,7 @@
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I9" s="6"/>
     </row>
@@ -1213,7 +1223,7 @@
         <v>55</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>72</v>
@@ -1234,7 +1244,7 @@
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G13" s="8"/>
     </row>
@@ -1253,7 +1263,7 @@
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G14" s="6"/>
     </row>
@@ -1272,7 +1282,7 @@
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G15" s="6"/>
     </row>

</xml_diff>